<commit_message>
recapturing alk crm data with header and setting top row in excel sheet to show header
</commit_message>
<xml_diff>
--- a/check sample work/TA/20201110 results summary both probes.xlsx
+++ b/check sample work/TA/20201110 results summary both probes.xlsx
@@ -7376,8 +7376,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>